<commit_message>
Quitada a Marina y siguiendo los diagramas
</commit_message>
<xml_diff>
--- a/docs/Diagrama tablas.xlsx
+++ b/docs/Diagrama tablas.xlsx
@@ -318,10 +318,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -721,13 +721,13 @@
       <c r="A9" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -883,17 +883,17 @@
       <c r="A25" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="15"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -1142,7 +1142,7 @@
       <c r="A57" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B57" s="14"/>
+      <c r="B57" s="15"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
@@ -1176,6 +1176,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A53:C53"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A33:F33"/>
     <mergeCell ref="A25:L25"/>
     <mergeCell ref="A1:C1"/>
@@ -1185,18 +1191,12 @@
     <mergeCell ref="A17:I17"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A21:D21"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A53:C53"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A57:B57"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="48" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;LDiagrama de tablas&amp;CDiagramas&amp;RHabilitación profesional</oddHeader>
-    <oddFooter>&amp;LEmiliano Gioria&amp;CMarina Ludi&amp;RAndrés Rico</oddFooter>
+    <oddFooter>&amp;LEmiliano Gioria&amp;RAndrés Rico</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>